<commit_message>
modified:   main.py 	new file:   massen_gesamt.xlsx 	modified:   massen_haltungen.csv 	modified:   massen_util/__inti__.py 	modified:   massen_util/pyexcel.py 	new file:   massen_util/src/.~lock.massen.xlsx# 	modified:   massen_util/src/massen.xlsx 	modified:   xml_parser/haltung.py 	modified:   xml_parser/xml_fixer.py
</commit_message>
<xml_diff>
--- a/massen_util/src/massen.xlsx
+++ b/massen_util/src/massen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Massen_Haltung" sheetId="1" state="visible" r:id="rId3"/>
@@ -44,8 +44,32 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">fq:
+geschätzt</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t xml:space="preserve">Massenermittlung</t>
   </si>
@@ -168,17 +192,37 @@
   </si>
   <si>
     <t xml:space="preserve">m³</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DN Zulauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DN Ablauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UGV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -378,8 +422,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,7 +459,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFA6CAF0"/>
+        <bgColor rgb="FFAFD095"/>
       </patternFill>
     </fill>
     <fill>
@@ -472,12 +530,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFE3E3E3"/>
         <bgColor rgb="FFF7F7F7"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="34">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -808,6 +872,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFF7F7F7"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFF7F7F7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF7F7F7"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFF7F7F7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FFF7F7F7"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair">
+        <color rgb="FFF7F7F7"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FFF7F7F7"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium">
+        <color rgb="FFF7F7F7"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -965,7 +1097,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -974,67 +1106,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1050,7 +1182,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="16" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="24" fillId="17" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1082,7 +1214,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="16" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="25" fillId="17" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1103,6 +1235,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="27" fillId="12" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1143,6 +1279,182 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="24" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="11" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="29" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="13" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="16" borderId="16" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="16" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="30" xfId="53" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="15" xfId="54" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="17" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="19" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="20" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="16" borderId="19" xfId="54" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="16" borderId="21" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="16" borderId="15" xfId="54" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="16" borderId="17" xfId="53" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="29" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="14" borderId="15" xfId="54" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="14" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="14" borderId="16" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="14" borderId="15" xfId="53" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="15" xfId="54" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="17" xfId="53" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="14" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="14" borderId="16" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="14" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="14" borderId="15" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="25" fillId="14" borderId="17" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="14" borderId="15" xfId="54" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="16" borderId="15" xfId="53" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="16" borderId="31" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="16" borderId="31" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="16" borderId="32" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="16" borderId="31" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="16" borderId="32" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="16" borderId="31" xfId="54" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="16" borderId="33" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1239,7 +1551,7 @@
       <rgbColor rgb="FFA6CAF0"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FF3333CC"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1374,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1390,9 +1702,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.27"/>
@@ -1400,7 +1712,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.55"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1737,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1448,7 +1760,7 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1793,7 @@
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
@@ -1601,7 +1913,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>35</v>
       </c>
@@ -3095,7 +3407,7 @@
       <c r="J31" s="22"/>
       <c r="K31" s="23"/>
       <c r="L31" s="24"/>
-      <c r="M31" s="10"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="23"/>
       <c r="O31" s="22"/>
       <c r="P31" s="23"/>
@@ -3106,36 +3418,36 @@
       <c r="U31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="40"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="40"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
-      <c r="T32" s="39"/>
-      <c r="U32" s="42"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="41"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="41"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="43"/>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="43"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="45"/>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3175,14 +3487,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="46"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3198,14 +3555,591 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="55"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="57" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="63"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="33"/>
+      <c r="B6" s="64" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C6" s="30" t="n">
+        <f aca="false">A6*B6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="30" t="n">
+        <f aca="false">1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="31" t="n">
+        <f aca="false">D6+G6+0.1</f>
+        <v>1.64</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H6" s="31" t="n">
+        <f aca="false">((F6/1000+2*G6)/2)^2*3.14*A6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="30" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="31" t="n">
+        <f aca="false">C6*I6</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="30" t="n">
+        <f aca="false">C6*E6-J6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="65" t="n">
+        <f aca="false">((0.05+F6/10000))</f>
+        <v>0.05</v>
+      </c>
+      <c r="M6" s="65" t="n">
+        <f aca="false">(F6/1000+2*G6)*0.15</f>
+        <v>0.012</v>
+      </c>
+      <c r="N6" s="65" t="n">
+        <f aca="false">(L6+M6)*C6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="30" t="n">
+        <f aca="false">(F6/1000+G6+0.3)*(B6)*A6-((F6/1000+2*G6)/2)^2*3.14*A6</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="30" t="n">
+        <f aca="false">K6-N6-O6-H6</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="66" t="n">
+        <f aca="false">2*A6*(E6-I6+0.05)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="33"/>
+      <c r="B7" s="64" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C7" s="30" t="n">
+        <f aca="false">A7*B7</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="30" t="n">
+        <f aca="false">1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="31" t="n">
+        <f aca="false">D7+G7+0.1</f>
+        <v>1.64</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H7" s="31" t="n">
+        <f aca="false">((F7/1000+2*G7)/2)^2*3.14*A7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="30" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <f aca="false">C7*I7</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="30" t="n">
+        <f aca="false">C7*E7-J7</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="65" t="n">
+        <f aca="false">((0.05+F7/10000))</f>
+        <v>0.05</v>
+      </c>
+      <c r="M7" s="65" t="n">
+        <f aca="false">(F7/1000+2*G7)*0.15</f>
+        <v>0.012</v>
+      </c>
+      <c r="N7" s="65" t="n">
+        <f aca="false">(L7+M7)*C7</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="30" t="n">
+        <f aca="false">(F7/1000+G7+0.3)*(B7)*A7-((F7/1000+2*G7)/2)^2*3.14*A7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="30" t="n">
+        <f aca="false">K7-N7-O7-H7</f>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="66" t="n">
+        <f aca="false">2*A7*(E7-I7+0.05)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="33"/>
+      <c r="B8" s="64" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C8" s="30" t="n">
+        <f aca="false">A8*B8</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="30" t="n">
+        <f aca="false">1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="E8" s="31" t="n">
+        <f aca="false">D8+G8+0.1</f>
+        <v>1.64</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H8" s="31" t="n">
+        <f aca="false">((F8/1000+2*G8)/2)^2*3.14*A8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="30" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J8" s="31" t="n">
+        <f aca="false">C8*I8</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="30" t="n">
+        <f aca="false">C8*E8-J8</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="65" t="n">
+        <f aca="false">((0.05+F8/10000))</f>
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="65" t="n">
+        <f aca="false">(F8/1000+2*G8)*0.15</f>
+        <v>0.012</v>
+      </c>
+      <c r="N8" s="65" t="n">
+        <f aca="false">(L8+M8)*C8</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="30" t="n">
+        <f aca="false">(F8/1000+G8+0.3)*(B8)*A8-((F8/1000+2*G8)/2)^2*3.14*A8</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="30" t="n">
+        <f aca="false">K8-N8-O8-H8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="66" t="n">
+        <f aca="false">2*A8*(E8-I8+0.05)</f>
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="66"/>
+    </row>
+    <row r="10" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="74"/>
+    </row>
+    <row r="11" s="75" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="76"/>
+      <c r="Q11" s="80"/>
+    </row>
+    <row r="12" s="75" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="65"/>
+      <c r="N12" s="65"/>
+      <c r="O12" s="76"/>
+      <c r="P12" s="76"/>
+      <c r="Q12" s="80"/>
+    </row>
+    <row r="13" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="74"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="63"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="63"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="62"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="51"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="63"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="83"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="83" t="n">
+        <f aca="false">SUM(C5:C16)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="87" t="n">
+        <f aca="false">SUM(H5:H16)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="84"/>
+      <c r="J17" s="87" t="n">
+        <f aca="false">SUM(J5:J16)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="83" t="n">
+        <f aca="false">SUM(K5:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="88"/>
+      <c r="M17" s="88"/>
+      <c r="N17" s="83" t="n">
+        <f aca="false">SUM(N5:N16)</f>
+        <v>0</v>
+      </c>
+      <c r="O17" s="83" t="n">
+        <f aca="false">SUM(O5:O16)</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="83" t="n">
+        <f aca="false">SUM(P5:P16)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="89" t="n">
+        <f aca="false">SUM(Q5:Q16)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3213,5 +4147,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   earth_filling/__inti__.py 	modified:   earth_filling/functionSet.py 	deleted:    earth_filling/vol_2polygon.py 	new file:   earth_filling/vol_polygon.py 	modified:   hydraulik/forge_inp.py 	modified:   main.py 	modified:   massen_util/__inti__.py 	modified:   massen_util/csv_creator.py 	modified:   massen_util/get_mass.py 	modified:   massen_util/merge_elements.py 	modified:   massen_util/pyexcel.py 	new file:   massen_util/src/.~lock.massen.xlsx# 	modified:   massen_util/src/massen.xlsx 	new file:   orientation/selected_columns.json 	modified:   server.py 	new file:   storage/output_xlsx_csv/massen_bauwerk.csv 	new file:   storage/output_xlsx_csv/massen_gesamt.xlsx 	new file:   storage/output_xlsx_csv/massen_haltungen.csv 	new file:   storage/output_xlsx_csv/massen_leitung.csv 	new file:   storage/output_xlsx_csv/massen_schacht.csv 	modified:   xml_parser/__init__.py 	modified:   xml_parser/bauwerk.py 	modified:   xml_parser/parse_all.py
</commit_message>
<xml_diff>
--- a/massen_util/src/massen.xlsx
+++ b/massen_util/src/massen.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Massen_Haltung" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Massen_Schacht" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Massen_Leitung" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Massen_Haltung" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Massen_Schacht" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Massen_Leitung" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Massen_Bauwerk" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="J9" authorId="0">
@@ -33,7 +34,8 @@
           <rPr>
             <sz val="10"/>
             <rFont val="Arial"/>
-            <family val="2"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">fq:
 geschätzt</t>
@@ -47,7 +49,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="D6" authorId="0">
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="61">
   <si>
     <t xml:space="preserve">Massenermittlung</t>
   </si>
@@ -210,6 +212,48 @@
   </si>
   <si>
     <t xml:space="preserve">Beton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bauwerke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Für Rechteck Volumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Für Trapez Volumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bauwerk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bauwerkart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breite OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laenge OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flaeche OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flaeche UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volumen 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volumen 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m³ (Rechteckig)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m³ (Trapez 1.5)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +266,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -418,11 +462,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -541,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="38">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -940,6 +979,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="medium">
+        <color rgb="FFF7F7F7"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="hair">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF7F7F7"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1097,7 +1172,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1354,7 +1429,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="28" fillId="14" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1370,7 +1445,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="30" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1455,6 +1530,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="23" fillId="16" borderId="33" xfId="53" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="16" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="16" borderId="37" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1573,130 +1668,24 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="6.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="6.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.84"/>
@@ -1708,7 +1697,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="7.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="9.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.55"/>
   </cols>
   <sheetData>
@@ -3483,17 +3472,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="46"/>
@@ -3551,17 +3540,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="48" t="s">
@@ -4149,4 +4138,224 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:T4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="90" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="90" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="92" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="93" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="P1:T1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>